<commit_message>
Implantado Misturados de Palpites
</commit_message>
<xml_diff>
--- a/DIA_DE_SORTE.xlsx
+++ b/DIA_DE_SORTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Meu Drive\LoteriasCaixaJogos\JOGOS\Resultados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Meu Drive\LoteriasCaixaSites\Loterias-GeradorBaseadoEmDigitos\GeradorBaseadoEmDigitosDiaDeSorte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EE10D-B235-4D54-8231-8620C5EE57DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55148E05-9002-48E9-82DF-DD6ED494F63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="444" windowWidth="17280" windowHeight="9072" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="DIA DE SORTE" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14585" uniqueCount="5842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14586" uniqueCount="5842">
   <si>
     <t>Concurso</t>
   </si>
@@ -17614,13 +17614,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17942,10 +17945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0EF237-0006-4F20-96DD-6728B25963DA}">
-  <dimension ref="A1:AH1041"/>
+  <dimension ref="A1:AH1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1028" workbookViewId="0">
-      <selection activeCell="J1041" sqref="J1041"/>
+    <sheetView tabSelected="1" topLeftCell="A1015" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:J1042"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -98130,6 +98133,41 @@
         <v>37</v>
       </c>
     </row>
+    <row r="1042" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1042">
+        <v>1041</v>
+      </c>
+      <c r="B1042" s="3">
+        <v>45736</v>
+      </c>
+      <c r="C1042">
+        <v>6</v>
+      </c>
+      <c r="D1042">
+        <v>9</v>
+      </c>
+      <c r="E1042">
+        <v>10</v>
+      </c>
+      <c r="F1042">
+        <v>14</v>
+      </c>
+      <c r="G1042">
+        <v>20</v>
+      </c>
+      <c r="H1042">
+        <v>22</v>
+      </c>
+      <c r="I1042">
+        <v>23</v>
+      </c>
+      <c r="J1042" t="s">
+        <v>5836</v>
+      </c>
+      <c r="K1042">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -98137,6 +98175,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -98144,15 +98191,6 @@
     <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-03-19T04:13:02+00:00</AtualizadoPeloTimerJobEm>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -98324,20 +98362,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03C591FA-4714-4C17-A356-DC7D36BA37AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0CE4A8-A4B4-44C5-B319-6698794A809E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03C591FA-4714-4C17-A356-DC7D36BA37AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>